<commit_message>
[ADD] type category + sorting
Signed-off-by: Alexandre Ferreira Benevides <alexandre.ferreira.benevides@gmail.com>
</commit_message>
<xml_diff>
--- a/ListeQuestions.xlsx
+++ b/ListeQuestions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandreferreirabenevides/Documents/LESIAQ/2020/MEC1010/Moodle_quiz_xml_creator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A5C519-BBAF-D64F-90A6-0B3E7D44D83B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27592406-7EC4-B147-90A7-6326AAA6D648}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pondération" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="73">
   <si>
     <t>ID Module</t>
   </si>
@@ -119,12 +119,6 @@
     <t>Vrai ou Faux</t>
   </si>
   <si>
-    <t>Réponse courte</t>
-  </si>
-  <si>
-    <t>Glisser-déposer sur une image</t>
-  </si>
-  <si>
     <t>Types de question dsponibles</t>
   </si>
   <si>
@@ -188,9 +182,6 @@
     <t>Section3</t>
   </si>
   <si>
-    <t>Question 1</t>
-  </si>
-  <si>
     <t>reponse 1</t>
   </si>
   <si>
@@ -221,14 +212,59 @@
     <t>Réponse5</t>
   </si>
   <si>
-    <t>Question 2</t>
+    <t>Question 1 choix multiple simple</t>
+  </si>
+  <si>
+    <t>Question 2 choix multiple checkbox</t>
+  </si>
+  <si>
+    <t>Question 3 vrai ou faux</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>Question 4 numérique</t>
+  </si>
+  <si>
+    <t>Numerique</t>
+  </si>
+  <si>
+    <t>Question 5 short answer</t>
+  </si>
+  <si>
+    <t>Reponse courte</t>
+  </si>
+  <si>
+    <t>Glisser-deposer sur une image</t>
+  </si>
+  <si>
+    <t>*Douche*</t>
+  </si>
+  <si>
+    <t>*extincteurs*</t>
+  </si>
+  <si>
+    <t>*Trousse*</t>
+  </si>
+  <si>
+    <t>*sortie de secours*</t>
+  </si>
+  <si>
+    <t>*Douche* *Trousse* *extincteurs* *sortie de secours*</t>
+  </si>
+  <si>
+    <t>Categories</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -292,8 +328,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFA9B7C6"/>
+      <name val="JetBrains Mono"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC7832"/>
+      <name val="JetBrains Mono"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -345,6 +396,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF4B084"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -561,7 +618,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -707,6 +764,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -716,10 +777,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1047,22 +1108,22 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.5" style="1"/>
     <col min="2" max="2" width="65" customWidth="1"/>
     <col min="3" max="3" width="11.5" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="33">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>1</v>
@@ -1077,12 +1138,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C2" s="22">
         <v>0.1</v>
@@ -1093,19 +1154,19 @@
       </c>
       <c r="E2" s="24">
         <f>SUM(E3:E5)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F2" s="24">
         <f>SUM(F3:F5)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C3" s="18">
         <v>0</v>
@@ -1123,12 +1184,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C4" s="18">
         <v>0.02</v>
@@ -1139,19 +1200,19 @@
       </c>
       <c r="E4" s="3">
         <f>COUNTIF(ListeQuestions!A:C,Pondération!A4)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="3">
         <f>COUNTIF(ListeQuestions!A:A,Pondération!A4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C5" s="19">
         <v>0.08</v>
@@ -1162,19 +1223,19 @@
       </c>
       <c r="E5" s="3">
         <f>COUNTIF(ListeQuestions!A:C,Pondération!A5)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="3">
         <f>COUNTIF(ListeQuestions!A:A,Pondération!A5)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="14" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C6" s="22">
         <v>0.4</v>
@@ -1192,12 +1253,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C7" s="18">
         <v>0.3</v>
@@ -1215,12 +1276,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C8" s="18">
         <v>0.05</v>
@@ -1238,12 +1299,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C9" s="19">
         <v>0.05</v>
@@ -1261,12 +1322,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C10" s="22">
         <v>0.4</v>
@@ -1284,12 +1345,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C11" s="18">
         <v>0.12</v>
@@ -1307,12 +1368,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C12" s="18">
         <v>0.12</v>
@@ -1330,12 +1391,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C13" s="18">
         <v>0.06</v>
@@ -1353,12 +1414,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" s="16" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C14" s="22">
         <v>0.1</v>
@@ -1371,17 +1432,17 @@
         <f>E15</f>
         <v>0</v>
       </c>
-      <c r="F14" s="66">
+      <c r="F14" s="63">
         <f>F15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="8"/>
@@ -1389,12 +1450,12 @@
         <f>COUNTIF(ListeQuestions!A:C,Pondération!A15)</f>
         <v>0</v>
       </c>
-      <c r="F15" s="67">
+      <c r="F15" s="64">
         <f>COUNTIF(ListeQuestions!A:A,Pondération!A15)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="B16" s="5"/>
       <c r="C16" s="21">
         <f>SUM(C14,C10,C6,C2)</f>
@@ -1404,7 +1465,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2">
       <c r="B17" s="5"/>
     </row>
   </sheetData>
@@ -1418,14 +1479,14 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:O118"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.5" style="40"/>
     <col min="2" max="3" width="11.5" style="41"/>
@@ -1436,16 +1497,16 @@
     <col min="10" max="16384" width="11.5" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F1" s="63" t="s">
+    <row r="1" spans="1:15" ht="16" thickBot="1">
+      <c r="F1" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="65"/>
-    </row>
-    <row r="2" spans="1:15" ht="33" x14ac:dyDescent="0.25">
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="67"/>
+    </row>
+    <row r="2" spans="1:15" ht="33">
       <c r="A2" s="25" t="s">
         <v>20</v>
       </c>
@@ -1477,129 +1538,178 @@
         <v>5</v>
       </c>
       <c r="K2" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="M2" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="N2" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="L2" s="30" t="s">
+      <c r="O2" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="M2" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="N2" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="O2" s="30" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="44"/>
+    </row>
+    <row r="3" spans="1:15" ht="16">
+      <c r="A3" s="44" t="s">
+        <v>5</v>
+      </c>
       <c r="B3" s="45"/>
       <c r="C3" s="45"/>
       <c r="D3" s="46" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>72</v>
       </c>
       <c r="F3" s="29"/>
     </row>
-    <row r="4" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="47"/>
+    <row r="4" spans="1:15" ht="16">
+      <c r="A4" s="47" t="s">
+        <v>7</v>
+      </c>
       <c r="B4" s="48"/>
       <c r="C4" s="48"/>
       <c r="D4" s="31" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E4" s="30" t="s">
         <v>23</v>
       </c>
       <c r="F4" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="31" t="s">
+      <c r="J4" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="H4" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="I4" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="J4" s="31" t="s">
-        <v>54</v>
-      </c>
       <c r="K4" s="30">
         <v>1</v>
       </c>
-      <c r="M4" s="30">
-        <v>1</v>
-      </c>
-      <c r="O4" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="47"/>
+    </row>
+    <row r="5" spans="1:15" ht="16">
+      <c r="A5" s="47" t="s">
+        <v>8</v>
+      </c>
       <c r="B5" s="48"/>
       <c r="C5" s="48"/>
       <c r="D5" s="31" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F5" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="G5" s="31" t="s">
+      <c r="J5" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="H5" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="I5" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="J5" s="31" t="s">
-        <v>54</v>
-      </c>
       <c r="K5" s="30">
         <v>0</v>
       </c>
       <c r="L5" s="30">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N5" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="16">
       <c r="A6" s="50"/>
       <c r="B6" s="51"/>
       <c r="C6" s="51"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
+      <c r="D6" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="68"/>
       <c r="I6" s="31"/>
       <c r="J6" s="31"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K6" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="16">
       <c r="A7" s="47"/>
       <c r="B7" s="48"/>
       <c r="C7" s="48"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="30"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D7" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="31">
+        <v>3</v>
+      </c>
+      <c r="G7" s="31"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="30">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="80">
       <c r="A8" s="47"/>
       <c r="B8" s="48"/>
       <c r="C8" s="48"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="49"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D8" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="68"/>
+      <c r="I8" s="31"/>
+      <c r="K8" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="L8" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="M8" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="N8" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="O8" s="30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="47"/>
       <c r="B9" s="48"/>
       <c r="C9" s="48"/>
@@ -1607,12 +1717,12 @@
       <c r="E9" s="30"/>
       <c r="F9" s="31"/>
       <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
+      <c r="H9" s="69"/>
       <c r="I9" s="31"/>
       <c r="J9" s="31"/>
       <c r="K9" s="31"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15">
       <c r="A10" s="47"/>
       <c r="B10" s="48"/>
       <c r="C10" s="48"/>
@@ -1620,11 +1730,11 @@
       <c r="E10" s="30"/>
       <c r="F10" s="49"/>
       <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
+      <c r="H10" s="69"/>
       <c r="I10" s="49"/>
       <c r="J10" s="49"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15">
       <c r="A11" s="47"/>
       <c r="B11" s="48"/>
       <c r="C11" s="48"/>
@@ -1632,11 +1742,11 @@
       <c r="E11" s="30"/>
       <c r="F11" s="49"/>
       <c r="G11" s="49"/>
-      <c r="H11" s="49"/>
+      <c r="H11" s="70"/>
       <c r="I11" s="49"/>
       <c r="J11" s="49"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15">
       <c r="A12" s="47"/>
       <c r="B12" s="48"/>
       <c r="C12" s="48"/>
@@ -1648,7 +1758,7 @@
       <c r="I12" s="31"/>
       <c r="J12" s="31"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15">
       <c r="A13" s="47"/>
       <c r="B13" s="48"/>
       <c r="C13" s="48"/>
@@ -1660,7 +1770,7 @@
       <c r="I13" s="49"/>
       <c r="J13" s="49"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15">
       <c r="A14" s="47"/>
       <c r="B14" s="48"/>
       <c r="C14" s="48"/>
@@ -1672,7 +1782,7 @@
       <c r="I14" s="31"/>
       <c r="J14" s="31"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15">
       <c r="A15" s="47"/>
       <c r="B15" s="48"/>
       <c r="C15" s="48"/>
@@ -1684,7 +1794,7 @@
       <c r="I15" s="49"/>
       <c r="J15" s="49"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15">
       <c r="A16" s="47"/>
       <c r="B16" s="48"/>
       <c r="C16" s="48"/>
@@ -1697,7 +1807,7 @@
       <c r="J16" s="31"/>
       <c r="K16" s="31"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11">
       <c r="A17" s="47"/>
       <c r="B17" s="48"/>
       <c r="C17" s="48"/>
@@ -1709,7 +1819,7 @@
       <c r="I17" s="31"/>
       <c r="J17" s="31"/>
     </row>
-    <row r="18" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="20">
       <c r="A18" s="47"/>
       <c r="B18" s="48"/>
       <c r="C18" s="48"/>
@@ -1722,7 +1832,7 @@
       <c r="J18" s="49"/>
       <c r="K18" s="53"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11">
       <c r="A19" s="47"/>
       <c r="B19" s="48"/>
       <c r="C19" s="48"/>
@@ -1734,7 +1844,7 @@
       <c r="I19" s="49"/>
       <c r="J19" s="49"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11">
       <c r="A20" s="47"/>
       <c r="B20" s="48"/>
       <c r="C20" s="48"/>
@@ -1746,7 +1856,7 @@
       <c r="I20" s="31"/>
       <c r="J20" s="31"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11">
       <c r="A21" s="47"/>
       <c r="B21" s="48"/>
       <c r="C21" s="48"/>
@@ -1757,7 +1867,7 @@
       <c r="H21" s="31"/>
       <c r="J21" s="49"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11">
       <c r="A22" s="47"/>
       <c r="B22" s="48"/>
       <c r="C22" s="48"/>
@@ -1769,7 +1879,7 @@
       <c r="I22" s="31"/>
       <c r="J22" s="49"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11">
       <c r="A23" s="47"/>
       <c r="B23" s="48"/>
       <c r="C23" s="48"/>
@@ -1781,7 +1891,7 @@
       <c r="I23" s="49"/>
       <c r="J23" s="49"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11">
       <c r="A24" s="47"/>
       <c r="B24" s="48"/>
       <c r="C24" s="48"/>
@@ -1793,7 +1903,7 @@
       <c r="I24" s="31"/>
       <c r="J24" s="31"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11">
       <c r="A25" s="47"/>
       <c r="B25" s="48"/>
       <c r="C25" s="48"/>
@@ -1805,7 +1915,7 @@
       <c r="I25" s="49"/>
       <c r="J25" s="49"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11">
       <c r="A26" s="47"/>
       <c r="B26" s="48"/>
       <c r="C26" s="48"/>
@@ -1817,7 +1927,7 @@
       <c r="I26" s="49"/>
       <c r="J26" s="49"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11">
       <c r="A27" s="44"/>
       <c r="B27" s="45"/>
       <c r="C27" s="45"/>
@@ -1825,7 +1935,7 @@
       <c r="E27" s="46"/>
       <c r="F27" s="29"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11">
       <c r="A28" s="47"/>
       <c r="B28" s="48"/>
       <c r="C28" s="48"/>
@@ -1833,14 +1943,14 @@
       <c r="E28" s="54"/>
       <c r="F28" s="32"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11">
       <c r="A29" s="47"/>
       <c r="B29" s="48"/>
       <c r="C29" s="48"/>
       <c r="D29" s="31"/>
       <c r="F29" s="32"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11">
       <c r="A30" s="50"/>
       <c r="B30" s="51"/>
       <c r="C30" s="51"/>
@@ -1848,7 +1958,7 @@
       <c r="E30" s="52"/>
       <c r="F30" s="33"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11">
       <c r="A31" s="55"/>
       <c r="B31" s="56"/>
       <c r="C31" s="56"/>
@@ -1856,7 +1966,7 @@
       <c r="E31" s="46"/>
       <c r="F31" s="29"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11">
       <c r="A32" s="47"/>
       <c r="B32" s="48"/>
       <c r="C32" s="48"/>
@@ -1864,7 +1974,7 @@
       <c r="E32" s="54"/>
       <c r="F32" s="32"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10">
       <c r="A33" s="47"/>
       <c r="B33" s="48"/>
       <c r="C33" s="48"/>
@@ -1872,7 +1982,7 @@
       <c r="E33" s="54"/>
       <c r="F33" s="32"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10">
       <c r="A34" s="57"/>
       <c r="B34" s="48"/>
       <c r="C34" s="48"/>
@@ -1880,7 +1990,7 @@
       <c r="E34" s="54"/>
       <c r="F34" s="32"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10">
       <c r="A35" s="47"/>
       <c r="B35" s="48"/>
       <c r="C35" s="48"/>
@@ -1888,7 +1998,7 @@
       <c r="E35" s="54"/>
       <c r="F35" s="32"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10">
       <c r="A36" s="47"/>
       <c r="B36" s="48"/>
       <c r="C36" s="48"/>
@@ -1896,7 +2006,7 @@
       <c r="E36" s="54"/>
       <c r="F36" s="32"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10">
       <c r="A37" s="47"/>
       <c r="B37" s="48"/>
       <c r="C37" s="48"/>
@@ -1904,7 +2014,7 @@
       <c r="E37" s="54"/>
       <c r="F37" s="32"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10">
       <c r="A38" s="47"/>
       <c r="B38" s="48"/>
       <c r="C38" s="48"/>
@@ -1912,7 +2022,7 @@
       <c r="E38" s="54"/>
       <c r="F38" s="32"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10">
       <c r="A39" s="50"/>
       <c r="B39" s="51"/>
       <c r="C39" s="51"/>
@@ -1920,7 +2030,7 @@
       <c r="E39" s="52"/>
       <c r="F39" s="33"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10">
       <c r="A40" s="47"/>
       <c r="B40" s="48"/>
       <c r="C40" s="48"/>
@@ -1928,7 +2038,7 @@
       <c r="E40" s="58"/>
       <c r="F40" s="34"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10">
       <c r="A41" s="47"/>
       <c r="B41" s="48"/>
       <c r="C41" s="48"/>
@@ -1936,14 +2046,14 @@
       <c r="E41" s="58"/>
       <c r="F41" s="34"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10">
       <c r="A42" s="47"/>
       <c r="B42" s="48"/>
       <c r="C42" s="48"/>
       <c r="D42" s="31"/>
       <c r="F42" s="34"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10">
       <c r="A43" s="50"/>
       <c r="B43" s="51"/>
       <c r="C43" s="51"/>
@@ -1951,16 +2061,16 @@
       <c r="E43" s="52"/>
       <c r="F43" s="33"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10">
       <c r="A44" s="59"/>
       <c r="D44" s="31"/>
       <c r="E44" s="60"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10">
       <c r="A45" s="59"/>
       <c r="D45" s="31"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10">
       <c r="D46" s="31"/>
       <c r="E46" s="30"/>
       <c r="F46" s="31"/>
@@ -1969,7 +2079,7 @@
       <c r="I46" s="31"/>
       <c r="J46" s="31"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10">
       <c r="D47" s="31"/>
       <c r="E47" s="30"/>
       <c r="F47" s="31"/>
@@ -1978,7 +2088,7 @@
       <c r="I47" s="31"/>
       <c r="J47" s="31"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10">
       <c r="D48" s="31"/>
       <c r="E48" s="30"/>
       <c r="F48" s="31"/>
@@ -1987,7 +2097,7 @@
       <c r="I48" s="31"/>
       <c r="J48" s="31"/>
     </row>
-    <row r="49" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="4:10">
       <c r="D49" s="31"/>
       <c r="E49" s="30"/>
       <c r="F49" s="31"/>
@@ -1996,7 +2106,7 @@
       <c r="I49" s="31"/>
       <c r="J49" s="31"/>
     </row>
-    <row r="50" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="4:10">
       <c r="D50" s="31"/>
       <c r="E50" s="30"/>
       <c r="F50" s="31"/>
@@ -2005,7 +2115,7 @@
       <c r="I50" s="31"/>
       <c r="J50" s="31"/>
     </row>
-    <row r="51" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="4:10">
       <c r="D51" s="31"/>
       <c r="E51" s="30"/>
       <c r="F51" s="31"/>
@@ -2014,7 +2124,7 @@
       <c r="I51" s="31"/>
       <c r="J51" s="31"/>
     </row>
-    <row r="52" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="4:10">
       <c r="D52" s="31"/>
       <c r="E52" s="30"/>
       <c r="F52" s="31"/>
@@ -2023,7 +2133,7 @@
       <c r="I52" s="31"/>
       <c r="J52" s="31"/>
     </row>
-    <row r="53" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="4:10">
       <c r="D53" s="31"/>
       <c r="E53" s="30"/>
       <c r="F53" s="31"/>
@@ -2032,7 +2142,7 @@
       <c r="I53" s="31"/>
       <c r="J53" s="31"/>
     </row>
-    <row r="54" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="4:10">
       <c r="D54" s="31"/>
       <c r="E54" s="30"/>
       <c r="F54" s="31"/>
@@ -2041,7 +2151,7 @@
       <c r="I54" s="31"/>
       <c r="J54" s="31"/>
     </row>
-    <row r="55" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="4:10">
       <c r="D55" s="31"/>
       <c r="E55" s="30"/>
       <c r="F55" s="31"/>
@@ -2050,7 +2160,7 @@
       <c r="I55" s="31"/>
       <c r="J55" s="31"/>
     </row>
-    <row r="56" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="4:10">
       <c r="D56" s="31"/>
       <c r="E56" s="30"/>
       <c r="F56" s="31"/>
@@ -2059,7 +2169,7 @@
       <c r="I56" s="31"/>
       <c r="J56" s="31"/>
     </row>
-    <row r="57" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="4:10">
       <c r="D57" s="31"/>
       <c r="E57" s="30"/>
       <c r="F57" s="31"/>
@@ -2068,7 +2178,7 @@
       <c r="I57" s="31"/>
       <c r="J57" s="31"/>
     </row>
-    <row r="58" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="4:10">
       <c r="D58" s="31"/>
       <c r="E58" s="30"/>
       <c r="F58" s="31"/>
@@ -2077,7 +2187,7 @@
       <c r="I58" s="31"/>
       <c r="J58" s="31"/>
     </row>
-    <row r="59" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="4:10">
       <c r="D59" s="31"/>
       <c r="E59" s="30"/>
       <c r="F59" s="31"/>
@@ -2086,7 +2196,7 @@
       <c r="I59" s="31"/>
       <c r="J59" s="31"/>
     </row>
-    <row r="60" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="4:10">
       <c r="D60" s="31"/>
       <c r="E60" s="30"/>
       <c r="F60" s="31"/>
@@ -2095,7 +2205,7 @@
       <c r="I60" s="31"/>
       <c r="J60" s="31"/>
     </row>
-    <row r="61" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="4:10">
       <c r="D61" s="31"/>
       <c r="E61" s="30"/>
       <c r="F61" s="31"/>
@@ -2104,7 +2214,7 @@
       <c r="I61" s="31"/>
       <c r="J61" s="31"/>
     </row>
-    <row r="62" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="4:10">
       <c r="D62" s="31"/>
       <c r="E62" s="30"/>
       <c r="F62" s="31"/>
@@ -2113,7 +2223,7 @@
       <c r="I62" s="31"/>
       <c r="J62" s="31"/>
     </row>
-    <row r="63" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="4:10">
       <c r="D63" s="31"/>
       <c r="E63" s="30"/>
       <c r="F63" s="31"/>
@@ -2122,7 +2232,7 @@
       <c r="I63" s="31"/>
       <c r="J63" s="31"/>
     </row>
-    <row r="64" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="4:10">
       <c r="D64" s="31"/>
       <c r="E64" s="30"/>
       <c r="F64" s="31"/>
@@ -2131,7 +2241,7 @@
       <c r="I64" s="31"/>
       <c r="J64" s="31"/>
     </row>
-    <row r="65" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="4:10">
       <c r="D65" s="31"/>
       <c r="E65" s="30"/>
       <c r="F65" s="31"/>
@@ -2140,7 +2250,7 @@
       <c r="I65" s="31"/>
       <c r="J65" s="31"/>
     </row>
-    <row r="66" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="4:10">
       <c r="D66" s="31"/>
       <c r="E66" s="30"/>
       <c r="F66" s="31"/>
@@ -2149,7 +2259,7 @@
       <c r="I66" s="31"/>
       <c r="J66" s="31"/>
     </row>
-    <row r="67" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="4:10">
       <c r="D67" s="31"/>
       <c r="E67" s="30"/>
       <c r="F67" s="31"/>
@@ -2158,7 +2268,7 @@
       <c r="I67" s="31"/>
       <c r="J67" s="31"/>
     </row>
-    <row r="68" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="4:10">
       <c r="D68" s="31"/>
       <c r="E68" s="30"/>
       <c r="F68" s="31"/>
@@ -2167,7 +2277,7 @@
       <c r="I68" s="31"/>
       <c r="J68" s="31"/>
     </row>
-    <row r="69" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="4:10">
       <c r="D69" s="31"/>
       <c r="E69" s="30"/>
       <c r="F69" s="31"/>
@@ -2176,7 +2286,7 @@
       <c r="I69" s="31"/>
       <c r="J69" s="31"/>
     </row>
-    <row r="70" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="4:10">
       <c r="D70" s="31"/>
       <c r="E70" s="30"/>
       <c r="F70" s="31"/>
@@ -2185,7 +2295,7 @@
       <c r="I70" s="31"/>
       <c r="J70" s="31"/>
     </row>
-    <row r="71" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="4:10">
       <c r="D71" s="31"/>
       <c r="E71" s="30"/>
       <c r="F71" s="31"/>
@@ -2194,7 +2304,7 @@
       <c r="I71" s="31"/>
       <c r="J71" s="31"/>
     </row>
-    <row r="72" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="72" spans="4:10">
       <c r="D72" s="31"/>
       <c r="E72" s="30"/>
       <c r="F72" s="31"/>
@@ -2203,7 +2313,7 @@
       <c r="I72" s="31"/>
       <c r="J72" s="31"/>
     </row>
-    <row r="73" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="4:10">
       <c r="D73" s="31"/>
       <c r="F73" s="31"/>
       <c r="G73" s="31"/>
@@ -2211,7 +2321,7 @@
       <c r="I73" s="31"/>
       <c r="J73" s="31"/>
     </row>
-    <row r="74" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="4:10">
       <c r="D74" s="31"/>
       <c r="E74" s="30"/>
       <c r="F74" s="31"/>
@@ -2220,7 +2330,7 @@
       <c r="I74" s="31"/>
       <c r="J74" s="31"/>
     </row>
-    <row r="75" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="75" spans="4:10">
       <c r="D75" s="31"/>
       <c r="E75" s="30"/>
       <c r="F75" s="31"/>
@@ -2229,7 +2339,7 @@
       <c r="I75" s="31"/>
       <c r="J75" s="31"/>
     </row>
-    <row r="76" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="76" spans="4:10">
       <c r="D76" s="31"/>
       <c r="E76" s="30"/>
       <c r="F76" s="31"/>
@@ -2238,7 +2348,7 @@
       <c r="I76" s="31"/>
       <c r="J76" s="31"/>
     </row>
-    <row r="77" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="4:10">
       <c r="D77" s="31"/>
       <c r="E77" s="30"/>
       <c r="F77" s="31"/>
@@ -2247,7 +2357,7 @@
       <c r="I77" s="31"/>
       <c r="J77" s="31"/>
     </row>
-    <row r="78" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="78" spans="4:10">
       <c r="D78" s="31"/>
       <c r="E78" s="30"/>
       <c r="F78" s="31"/>
@@ -2256,7 +2366,7 @@
       <c r="I78" s="31"/>
       <c r="J78" s="31"/>
     </row>
-    <row r="79" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="79" spans="4:10">
       <c r="D79" s="31"/>
       <c r="E79" s="30"/>
       <c r="F79" s="31"/>
@@ -2265,7 +2375,7 @@
       <c r="I79" s="31"/>
       <c r="J79" s="31"/>
     </row>
-    <row r="80" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="80" spans="4:10">
       <c r="D80" s="31"/>
       <c r="E80" s="30"/>
       <c r="F80" s="31"/>
@@ -2274,7 +2384,7 @@
       <c r="I80" s="31"/>
       <c r="J80" s="31"/>
     </row>
-    <row r="81" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="4:11">
       <c r="D81" s="31"/>
       <c r="E81" s="30"/>
       <c r="F81" s="31"/>
@@ -2283,7 +2393,7 @@
       <c r="I81" s="31"/>
       <c r="J81" s="31"/>
     </row>
-    <row r="82" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="4:11">
       <c r="D82" s="31"/>
       <c r="E82" s="30"/>
       <c r="F82" s="31"/>
@@ -2292,7 +2402,7 @@
       <c r="I82" s="31"/>
       <c r="J82" s="31"/>
     </row>
-    <row r="83" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="4:11">
       <c r="D83" s="31"/>
       <c r="E83" s="30"/>
       <c r="F83" s="31"/>
@@ -2301,7 +2411,7 @@
       <c r="I83" s="31"/>
       <c r="J83" s="31"/>
     </row>
-    <row r="84" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="4:11">
       <c r="D84" s="31"/>
       <c r="E84" s="30"/>
       <c r="F84" s="31"/>
@@ -2310,7 +2420,7 @@
       <c r="I84" s="31"/>
       <c r="J84" s="31"/>
     </row>
-    <row r="85" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="4:11">
       <c r="D85" s="31"/>
       <c r="E85" s="30"/>
       <c r="F85" s="31"/>
@@ -2319,7 +2429,7 @@
       <c r="I85" s="31"/>
       <c r="J85" s="31"/>
     </row>
-    <row r="86" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="4:11">
       <c r="D86" s="31"/>
       <c r="E86" s="30"/>
       <c r="F86" s="31"/>
@@ -2328,7 +2438,7 @@
       <c r="I86" s="31"/>
       <c r="J86" s="31"/>
     </row>
-    <row r="87" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="4:11">
       <c r="D87" s="31"/>
       <c r="E87" s="30"/>
       <c r="F87" s="31"/>
@@ -2337,7 +2447,7 @@
       <c r="I87" s="31"/>
       <c r="J87" s="31"/>
     </row>
-    <row r="88" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="4:11">
       <c r="D88" s="31"/>
       <c r="E88" s="30"/>
       <c r="F88" s="31"/>
@@ -2346,48 +2456,48 @@
       <c r="I88" s="31"/>
       <c r="J88" s="31"/>
     </row>
-    <row r="89" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="89" spans="4:11">
       <c r="D89" s="31"/>
       <c r="E89" s="30"/>
     </row>
-    <row r="90" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="90" spans="4:11">
       <c r="D90" s="31"/>
       <c r="E90" s="30"/>
       <c r="K90" s="35"/>
     </row>
-    <row r="91" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="4:11">
       <c r="D91" s="31"/>
       <c r="E91" s="30"/>
       <c r="K91" s="35"/>
     </row>
-    <row r="92" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="92" spans="4:11">
       <c r="D92" s="31"/>
       <c r="E92" s="30"/>
       <c r="K92" s="35"/>
     </row>
-    <row r="93" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="93" spans="4:11">
       <c r="D93" s="31"/>
       <c r="E93" s="30"/>
     </row>
-    <row r="94" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="94" spans="4:11">
       <c r="D94" s="31"/>
       <c r="E94" s="30"/>
       <c r="K94" s="35"/>
     </row>
-    <row r="95" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="95" spans="4:11">
       <c r="D95" s="31"/>
       <c r="E95" s="30"/>
     </row>
-    <row r="96" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="96" spans="4:11">
       <c r="D96" s="31"/>
       <c r="E96" s="30"/>
     </row>
-    <row r="97" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="97" spans="4:10">
       <c r="D97" s="31"/>
       <c r="E97" s="30"/>
       <c r="F97" s="30"/>
     </row>
-    <row r="98" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="98" spans="4:10">
       <c r="D98" s="31"/>
       <c r="E98" s="30"/>
       <c r="F98" s="31"/>
@@ -2396,7 +2506,7 @@
       <c r="I98" s="31"/>
       <c r="J98" s="31"/>
     </row>
-    <row r="99" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="99" spans="4:10">
       <c r="D99" s="31"/>
       <c r="E99" s="30"/>
       <c r="F99" s="31"/>
@@ -2405,61 +2515,61 @@
       <c r="I99" s="31"/>
       <c r="J99" s="31"/>
     </row>
-    <row r="100" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="100" spans="4:10">
       <c r="D100" s="30"/>
     </row>
-    <row r="101" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="101" spans="4:10">
       <c r="D101" s="30"/>
     </row>
-    <row r="102" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="102" spans="4:10">
       <c r="D102" s="30"/>
     </row>
-    <row r="103" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="103" spans="4:10">
       <c r="D103" s="30"/>
     </row>
-    <row r="104" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="104" spans="4:10">
       <c r="D104" s="30"/>
     </row>
-    <row r="105" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="105" spans="4:10">
       <c r="D105" s="30"/>
     </row>
-    <row r="106" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="106" spans="4:10">
       <c r="D106" s="30"/>
     </row>
-    <row r="107" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="107" spans="4:10">
       <c r="D107" s="49"/>
     </row>
-    <row r="108" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="108" spans="4:10">
       <c r="D108" s="49"/>
     </row>
-    <row r="109" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="109" spans="4:10">
       <c r="D109" s="49"/>
     </row>
-    <row r="110" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="110" spans="4:10">
       <c r="D110" s="49"/>
     </row>
-    <row r="111" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="111" spans="4:10">
       <c r="D111" s="49"/>
     </row>
-    <row r="112" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="112" spans="4:10">
       <c r="D112" s="49"/>
     </row>
-    <row r="113" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="4:4">
       <c r="D113" s="49"/>
     </row>
-    <row r="114" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="4:4">
       <c r="D114" s="49"/>
     </row>
-    <row r="115" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="4:4">
       <c r="D115" s="49"/>
     </row>
-    <row r="116" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="4:4">
       <c r="D116" s="49"/>
     </row>
-    <row r="117" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="4:4">
       <c r="D117" s="49"/>
     </row>
-    <row r="118" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="118" spans="4:4">
       <c r="D118" s="49"/>
     </row>
   </sheetData>
@@ -2493,7 +2603,7 @@
           <x14:formula1>
             <xm:f>'Types de questions isponibles'!$A$2:$A$10</xm:f>
           </x14:formula1>
-          <xm:sqref>E4:E26 E46:E72 E74:E99</xm:sqref>
+          <xm:sqref>E74:E99 E46:E72 E3:E26</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2509,7 +2619,7 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="90.1640625" customWidth="1"/>
     <col min="2" max="2" width="15.1640625" customWidth="1"/>
@@ -2526,42 +2636,42 @@
     <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="32">
       <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="D1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="E1" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="G1" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="I1" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="J1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:13" ht="16">
       <c r="A4" t="str">
         <f>ListeQuestions!D4</f>
-        <v>Question 1</v>
+        <v>Question 1 choix multiple simple</v>
       </c>
       <c r="B4" t="str">
         <f>VLOOKUP(ListeQuestions!E4,'Types de questions isponibles'!$A$3:$B$7,2,)</f>
@@ -2608,14 +2718,14 @@
         <v>Choix multiple simple</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="16">
       <c r="A5" t="str">
         <f>ListeQuestions!D5</f>
-        <v>Question 2</v>
+        <v>Question 2 choix multiple checkbox</v>
       </c>
       <c r="B5" t="str">
         <f>VLOOKUP(ListeQuestions!E5,'Types de questions isponibles'!$A$3:$B$7,2,)</f>
-        <v>U</v>
+        <v>M</v>
       </c>
       <c r="C5" s="30" t="str">
         <f>ListeQuestions!F5</f>
@@ -2655,28 +2765,28 @@
       </c>
       <c r="M5" t="str">
         <f>ListeQuestions!E5</f>
-        <v>Choix multiple simple</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6">
+        <v>Choix multiple checkbox</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="str">
         <f>ListeQuestions!D6</f>
-        <v>0</v>
-      </c>
-      <c r="B6" t="e">
+        <v>Question 3 vrai ou faux</v>
+      </c>
+      <c r="B6" t="str">
         <f>VLOOKUP(ListeQuestions!E6,'Types de questions isponibles'!$A$3:$B$7,2,)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C6" s="30">
+        <v>U</v>
+      </c>
+      <c r="C6" s="30" t="str">
         <f>ListeQuestions!F6</f>
-        <v>0</v>
+        <v>true</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="30" t="str">
         <f>ListeQuestions!G6</f>
-        <v>0</v>
+        <v>false</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -2701,17 +2811,17 @@
       </c>
       <c r="L6">
         <f>ListeQuestions!K6</f>
-        <v>0</v>
-      </c>
-      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="M6" t="str">
         <f>ListeQuestions!E6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7">
+        <v>Vrai ou Faux</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="str">
         <f>ListeQuestions!D7</f>
-        <v>0</v>
+        <v>Question 4 numérique</v>
       </c>
       <c r="B7" t="e">
         <f>VLOOKUP(ListeQuestions!E7,'Types de questions isponibles'!$A$3:$B$7,2,)</f>
@@ -2732,21 +2842,21 @@
       <c r="K7" s="62"/>
       <c r="L7">
         <f>ListeQuestions!K7</f>
-        <v>0</v>
-      </c>
-      <c r="M7">
+        <v>1024</v>
+      </c>
+      <c r="M7" t="str">
         <f>ListeQuestions!E7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8">
+        <v>Numerique</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="str">
         <f>ListeQuestions!D8</f>
-        <v>0</v>
-      </c>
-      <c r="B8" t="e">
+        <v>Question 5 short answer</v>
+      </c>
+      <c r="B8" t="str">
         <f>VLOOKUP(ListeQuestions!E8,'Types de questions isponibles'!$A$3:$B$7,2,)</f>
-        <v>#N/A</v>
+        <v>M</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -2761,16 +2871,16 @@
         <v>1</v>
       </c>
       <c r="K8" s="62"/>
-      <c r="L8">
-        <f>ListeQuestions!K8</f>
-        <v>0</v>
-      </c>
-      <c r="M8">
+      <c r="L8" t="str">
+        <f>ListeQuestions!L8</f>
+        <v>*Douche*</v>
+      </c>
+      <c r="M8" t="str">
         <f>ListeQuestions!E8</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+        <v>Reponse courte</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9">
         <f>ListeQuestions!D9</f>
         <v>0</v>
@@ -2820,7 +2930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13">
       <c r="A10">
         <f>ListeQuestions!D10</f>
         <v>0</v>
@@ -2851,7 +2961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13">
       <c r="A11">
         <f>ListeQuestions!D11</f>
         <v>0</v>
@@ -2882,7 +2992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13">
       <c r="A12">
         <f>ListeQuestions!D12</f>
         <v>0</v>
@@ -2932,7 +3042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13">
       <c r="A13">
         <f>ListeQuestions!D13</f>
         <v>0</v>
@@ -2963,7 +3073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13">
       <c r="A14">
         <f>ListeQuestions!D14</f>
         <v>0</v>
@@ -3013,7 +3123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13">
       <c r="A15">
         <f>ListeQuestions!D15</f>
         <v>0</v>
@@ -3044,7 +3154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13">
       <c r="A16">
         <f>ListeQuestions!D16</f>
         <v>0</v>
@@ -3094,7 +3204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13">
       <c r="A17">
         <f>ListeQuestions!D17</f>
         <v>0</v>
@@ -3144,7 +3254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13">
       <c r="A18">
         <f>ListeQuestions!D18</f>
         <v>0</v>
@@ -3175,7 +3285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13">
       <c r="A19">
         <f>ListeQuestions!D19</f>
         <v>0</v>
@@ -3206,7 +3316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="96" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13">
       <c r="A20">
         <f>ListeQuestions!D20</f>
         <v>0</v>
@@ -3256,7 +3366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13">
       <c r="A21">
         <f>ListeQuestions!D21</f>
         <v>0</v>
@@ -3306,7 +3416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13">
       <c r="A22">
         <f>ListeQuestions!D22</f>
         <v>0</v>
@@ -3337,7 +3447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13">
       <c r="A23">
         <f>ListeQuestions!D23</f>
         <v>0</v>
@@ -3376,7 +3486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13">
       <c r="A24">
         <f>ListeQuestions!D24</f>
         <v>0</v>
@@ -3426,7 +3536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13">
       <c r="A25">
         <f>ListeQuestions!D25</f>
         <v>0</v>
@@ -3457,7 +3567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13">
       <c r="A26">
         <f>ListeQuestions!D26</f>
         <v>0</v>
@@ -3496,7 +3606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13">
       <c r="A27">
         <f>ListeQuestions!D27</f>
         <v>0</v>
@@ -3515,7 +3625,7 @@
       </c>
       <c r="K27" s="62"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13">
       <c r="A28">
         <f>ListeQuestions!D28</f>
         <v>0</v>
@@ -3534,7 +3644,7 @@
       </c>
       <c r="K28" s="62"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13">
       <c r="A29">
         <f>ListeQuestions!D29</f>
         <v>0</v>
@@ -3553,83 +3663,83 @@
       </c>
       <c r="K29" s="62"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13">
       <c r="K30" s="62"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13">
       <c r="A31">
         <f>ListeQuestions!D31</f>
         <v>0</v>
       </c>
       <c r="K31" s="62"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13">
       <c r="A32">
         <f>ListeQuestions!D32</f>
         <v>0</v>
       </c>
       <c r="K32" s="62"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13">
       <c r="A33">
         <f>ListeQuestions!D33</f>
         <v>0</v>
       </c>
       <c r="K33" s="62"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13">
       <c r="A34">
         <f>ListeQuestions!D34</f>
         <v>0</v>
       </c>
       <c r="K34" s="62"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13">
       <c r="K35" s="62"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13">
       <c r="K36" s="62"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13">
       <c r="K37" s="62"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13">
       <c r="K38" s="62"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13">
       <c r="K39" s="62"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13">
       <c r="A40">
         <f>ListeQuestions!D40</f>
         <v>0</v>
       </c>
       <c r="K40" s="62"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13">
       <c r="K41" s="62"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13">
       <c r="A42">
         <f>ListeQuestions!D42</f>
         <v>0</v>
       </c>
       <c r="K42" s="62"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13">
       <c r="A43">
         <f>ListeQuestions!D43</f>
         <v>0</v>
       </c>
       <c r="K43" s="62"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13">
       <c r="K44" s="62"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13">
       <c r="K45" s="62"/>
     </row>
-    <row r="46" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13">
       <c r="A46">
         <f>ListeQuestions!D46</f>
         <v>0</v>
@@ -3656,7 +3766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13">
       <c r="A47">
         <f>ListeQuestions!D47</f>
         <v>0</v>
@@ -3683,7 +3793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13">
       <c r="A48">
         <f>ListeQuestions!D48</f>
         <v>0</v>
@@ -3714,7 +3824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13">
       <c r="A49">
         <f>ListeQuestions!D49</f>
         <v>0</v>
@@ -3741,7 +3851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13">
       <c r="A50">
         <f>ListeQuestions!D50</f>
         <v>0</v>
@@ -3764,7 +3874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13">
       <c r="A51">
         <f>ListeQuestions!D51</f>
         <v>0</v>
@@ -3783,7 +3893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13">
       <c r="A52">
         <f>ListeQuestions!D52</f>
         <v>0</v>
@@ -3806,7 +3916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13">
       <c r="A53">
         <f>ListeQuestions!D53</f>
         <v>0</v>
@@ -3837,7 +3947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13">
       <c r="A54">
         <f>ListeQuestions!D54</f>
         <v>0</v>
@@ -3871,7 +3981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13">
       <c r="A55">
         <f>ListeQuestions!D55</f>
         <v>0</v>
@@ -3902,7 +4012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13">
       <c r="A56">
         <f>ListeQuestions!D56</f>
         <v>0</v>
@@ -3929,7 +4039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13">
       <c r="A57">
         <f>ListeQuestions!D57</f>
         <v>0</v>
@@ -3960,7 +4070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13">
       <c r="A58">
         <f>ListeQuestions!D58</f>
         <v>0</v>
@@ -3987,7 +4097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13">
       <c r="A59">
         <f>ListeQuestions!D59</f>
         <v>0</v>
@@ -4014,7 +4124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13">
       <c r="A60">
         <f>ListeQuestions!D60</f>
         <v>0</v>
@@ -4041,7 +4151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13">
       <c r="A61">
         <f>ListeQuestions!D61</f>
         <v>0</v>
@@ -4072,7 +4182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13">
       <c r="A62">
         <f>ListeQuestions!D62</f>
         <v>0</v>
@@ -4091,7 +4201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13">
       <c r="A63">
         <f>ListeQuestions!D63</f>
         <v>0</v>
@@ -4125,7 +4235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13">
       <c r="C64" s="30">
         <f>ListeQuestions!F64</f>
         <v>0</v>
@@ -4140,7 +4250,7 @@
       </c>
       <c r="K64" s="62"/>
     </row>
-    <row r="65" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13">
       <c r="A65">
         <f>ListeQuestions!D65</f>
         <v>0</v>
@@ -4159,7 +4269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13">
       <c r="A66">
         <f>ListeQuestions!D66</f>
         <v>0</v>
@@ -4178,7 +4288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13">
       <c r="A67">
         <f>ListeQuestions!D67</f>
         <v>0</v>
@@ -4197,7 +4307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13">
       <c r="A68">
         <f>ListeQuestions!D68</f>
         <v>0</v>
@@ -4216,7 +4326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13">
       <c r="A69">
         <f>ListeQuestions!D69</f>
         <v>0</v>
@@ -4243,7 +4353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13">
       <c r="A70">
         <f>ListeQuestions!D70</f>
         <v>0</v>
@@ -4270,7 +4380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13">
       <c r="A71">
         <f>ListeQuestions!D71</f>
         <v>0</v>
@@ -4289,7 +4399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13">
       <c r="A72">
         <f>ListeQuestions!D72</f>
         <v>0</v>
@@ -4323,7 +4433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13">
       <c r="C73" s="30">
         <f>ListeQuestions!F73</f>
         <v>0</v>
@@ -4334,7 +4444,7 @@
       </c>
       <c r="K73" s="62"/>
     </row>
-    <row r="74" spans="1:13" ht="128" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13">
       <c r="A74">
         <f>ListeQuestions!D74</f>
         <v>0</v>
@@ -4353,7 +4463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:13" ht="160" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13">
       <c r="A75">
         <f>ListeQuestions!D75</f>
         <v>0</v>
@@ -4372,7 +4482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:13" ht="144" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13">
       <c r="A76">
         <f>ListeQuestions!D76</f>
         <v>0</v>
@@ -4391,7 +4501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:13" ht="96" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:13">
       <c r="A77">
         <f>ListeQuestions!D77</f>
         <v>0</v>
@@ -4410,7 +4520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:13" ht="96" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:13">
       <c r="A78">
         <f>ListeQuestions!D78</f>
         <v>0</v>
@@ -4429,7 +4539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:13">
       <c r="A79">
         <f>ListeQuestions!D79</f>
         <v>0</v>
@@ -4448,7 +4558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:13">
       <c r="A80">
         <f>ListeQuestions!D80</f>
         <v>0</v>
@@ -4486,7 +4596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13">
       <c r="A81">
         <f>ListeQuestions!D81</f>
         <v>0</v>
@@ -4524,7 +4634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:13">
       <c r="A82">
         <f>ListeQuestions!D82</f>
         <v>0</v>
@@ -4562,7 +4672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:13">
       <c r="A83">
         <f>ListeQuestions!D83</f>
         <v>0</v>
@@ -4600,7 +4710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13">
       <c r="A84">
         <f>ListeQuestions!D84</f>
         <v>0</v>
@@ -4619,7 +4729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13">
       <c r="A85">
         <f>ListeQuestions!D85</f>
         <v>0</v>
@@ -4638,7 +4748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:13">
       <c r="A86">
         <f>ListeQuestions!D86</f>
         <v>0</v>
@@ -4657,7 +4767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:13">
       <c r="A87">
         <f>ListeQuestions!D87</f>
         <v>0</v>
@@ -4676,7 +4786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:13">
       <c r="A88">
         <f>ListeQuestions!D88</f>
         <v>0</v>
@@ -4695,7 +4805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:13">
       <c r="A89">
         <f>ListeQuestions!D89</f>
         <v>0</v>
@@ -4710,7 +4820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:13">
       <c r="A90">
         <f>ListeQuestions!D90</f>
         <v>0</v>
@@ -4729,7 +4839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:13">
       <c r="A91">
         <f>ListeQuestions!D91</f>
         <v>0</v>
@@ -4748,7 +4858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:13">
       <c r="A92">
         <f>ListeQuestions!D92</f>
         <v>0</v>
@@ -4767,7 +4877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:13">
       <c r="A93">
         <f>ListeQuestions!D93</f>
         <v>0</v>
@@ -4786,7 +4896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:13">
       <c r="A94">
         <f>ListeQuestions!D94</f>
         <v>0</v>
@@ -4805,7 +4915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:13">
       <c r="A95">
         <f>ListeQuestions!D95</f>
         <v>0</v>
@@ -4824,7 +4934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:13">
       <c r="A96">
         <f>ListeQuestions!D96</f>
         <v>0</v>
@@ -4843,7 +4953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:13">
       <c r="A97">
         <f>ListeQuestions!D97</f>
         <v>0</v>
@@ -4862,7 +4972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:13">
       <c r="A98">
         <f>ListeQuestions!D98</f>
         <v>0</v>
@@ -4900,7 +5010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:13">
       <c r="A99">
         <f>ListeQuestions!D99</f>
         <v>0</v>
@@ -4946,57 +5056,67 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D6865BF-791E-FB48-9E31-68974FADC4BD}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="40.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="36" t="s">
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="37" t="s">
         <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="38" t="s">
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" s="39" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16">
       <c r="A7" s="61" t="s">
-        <v>27</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="71" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -5006,25 +5126,11 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100447C80396883E44C97F93366B537FD40" ma:contentTypeVersion="3" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="093339f7b61bf79c62240caa7cde7d44">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d3e7a6ef-71bd-4131-9933-e0e605c48bb6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2edb3710819c013f300815b31e66b3f8" ns2:_="">
     <xsd:import namespace="d3e7a6ef-71bd-4131-9933-e0e605c48bb6"/>
@@ -5162,31 +5268,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDDE28AE-235B-46FA-B82A-F729CA567D2E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d3e7a6ef-71bd-4131-9933-e0e605c48bb6"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49B625F2-1A48-4E1D-A67F-02019883CB85}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D35BC84-F260-48D9-82A9-C0465F544B54}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5202,4 +5299,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49B625F2-1A48-4E1D-A67F-02019883CB85}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDDE28AE-235B-46FA-B82A-F729CA567D2E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d3e7a6ef-71bd-4131-9933-e0e605c48bb6"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>